<commit_message>
added total keywords to note df where particular value is not present
</commit_message>
<xml_diff>
--- a/output/0c710442-6047-497d-ba64-d9c31122e53b/0c710442-6047-497d-ba64-d9c31122e53b_notes_cropped_df.xlsx
+++ b/output/0c710442-6047-497d-ba64-d9c31122e53b/0c710442-6047-497d-ba64-d9c31122e53b_notes_cropped_df.xlsx
@@ -31,13 +31,14 @@
     <sheet name="4_7_fd791fd0-d8c8-32" sheetId="22" r:id="rId22"/>
     <sheet name="4_7_b1818398-7624-37" sheetId="23" r:id="rId23"/>
     <sheet name="4_7_412c019a-25e7-31" sheetId="24" r:id="rId24"/>
+    <sheet name="4_7_d493819c-94d0-30" sheetId="25" r:id="rId25"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="350">
   <si>
     <t>6. Cash and short-term deposits</t>
   </si>
@@ -3014,7 +3015,7 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3067,6 +3068,153 @@
       </c>
       <c r="C5" t="s">
         <v>213</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>186</v>
+      </c>
+      <c r="B6" t="s">
+        <v>192</v>
+      </c>
+      <c r="C6" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B7" t="s">
+        <v>209</v>
+      </c>
+      <c r="C7" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>204</v>
+      </c>
+      <c r="B8" t="s">
+        <v>210</v>
+      </c>
+      <c r="C8" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>205</v>
+      </c>
+      <c r="B9" t="s">
+        <v>195</v>
+      </c>
+      <c r="C9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>206</v>
+      </c>
+      <c r="B10" t="s">
+        <v>211</v>
+      </c>
+      <c r="C10" t="s">
+        <v>216</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>218</v>
+      </c>
+      <c r="B5" t="s">
+        <v>220</v>
+      </c>
+      <c r="C5" t="s">
+        <v>222</v>
+      </c>
+      <c r="D5" t="s">
+        <v>224</v>
+      </c>
+      <c r="E5" t="s">
+        <v>226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>